<commit_message>
poprawa nazw wstawianych w imporcie i baz niestandardowych, poprawa bledu pokreslen w etykiecie OT dla np bloku budynku
</commit_message>
<xml_diff>
--- a/raport/szablon_raport_importu.xlsx
+++ b/raport/szablon_raport_importu.xlsx
@@ -15,7 +15,7 @@
     <sheet name="QMapa_import" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">QMapa_import!$A:$I</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">QMapa_import!$A:$H</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
   <si>
     <t>Lp.</t>
   </si>
@@ -47,9 +47,6 @@
 obiektów</t>
   </si>
   <si>
-    <t>Typ geometrii</t>
-  </si>
-  <si>
     <t>pierwsze</t>
   </si>
   <si>
@@ -62,41 +59,9 @@
     <t>Liczba obiektów</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Plik: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>Plik_bdot500.gml</t>
-    </r>
-  </si>
-  <si>
     <t>W tym wersje</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Data i czas importu </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>RRRR-MM-DD gg:mm:ss</t>
-    </r>
-  </si>
-  <si>
     <t>© 2022 GEOXY sp. z o.o.</t>
   </si>
   <si>
@@ -119,13 +84,19 @@
   </si>
   <si>
     <t xml:space="preserve">Obiekty niestandardowe, baza: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plik: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data i czas importu: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -293,32 +264,24 @@
     <font>
       <b/>
       <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <b/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
       <sz val="6"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="28">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -462,6 +425,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFEF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F8FC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4F9F1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -723,30 +704,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="24" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
@@ -762,50 +737,38 @@
     <xf numFmtId="3" fontId="1" fillId="18" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="23" fillId="18" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="22" fillId="18" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="23" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="22" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="24" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -819,7 +782,7 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -840,14 +803,35 @@
     <xf numFmtId="0" fontId="21" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -855,11 +839,17 @@
     <xf numFmtId="3" fontId="1" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="23" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="22" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="23" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="22" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -867,10 +857,10 @@
     <xf numFmtId="0" fontId="1" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="23" fillId="18" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="22" fillId="18" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="23" fillId="18" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="22" fillId="18" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -879,17 +869,8 @@
     <xf numFmtId="0" fontId="1" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -940,6 +921,12 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF4F9F1"/>
+      <color rgb="FFF2F8FC"/>
+      <color rgb="FFF5FAFD"/>
+      <color rgb="FFECF4FA"/>
+      <color rgb="FFEAF3FA"/>
+      <color rgb="FFFFFFEF"/>
       <color rgb="FFFFFFCC"/>
       <color rgb="FF0000CC"/>
     </mruColors>
@@ -959,14 +946,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>361295</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>2627</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>387569</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>387568</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>8540</xdr:rowOff>
     </xdr:to>
@@ -975,7 +962,7 @@
         <xdr:cNvPr id="2" name="Obraz 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15A37402-D866-0FDD-4B11-9268CBD4FA76}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15A37402-D866-0FDD-4B11-9268CBD4FA76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1301,377 +1288,399 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="3" customWidth="1"/>
-    <col min="4" max="5" width="11.6640625" style="4" customWidth="1"/>
-    <col min="6" max="9" width="11.6640625" style="10" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="4" width="11.6640625" style="3" customWidth="1"/>
+    <col min="5" max="8" width="11.6640625" style="8" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="23" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="12"/>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="14"/>
-    </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="44"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="57" t="s">
+      <c r="F9" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="49"/>
+    </row>
+    <row r="10" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="35"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="39"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+    </row>
+    <row r="13" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="41"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+    </row>
+    <row r="15" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B16" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C16" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="50"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="E17" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="49"/>
+    </row>
+    <row r="18" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="20"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+    </row>
+    <row r="19" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="39"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+    </row>
+    <row r="21" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="42"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+    </row>
+    <row r="23" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="47" t="s">
+      <c r="D24" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="57"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="15" t="s">
+      <c r="E24" s="10"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="56"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="16" t="s">
+      <c r="G25" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H25" s="49"/>
+    </row>
+    <row r="26" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+    </row>
+    <row r="28" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="39"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+    </row>
+    <row r="29" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="43"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+    </row>
+    <row r="31" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="48"/>
-    </row>
-    <row r="10" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="9" t="s">
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+    </row>
+    <row r="33" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="52"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+    </row>
+    <row r="34" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="26"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+    </row>
+    <row r="35" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-    </row>
-    <row r="13" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="47" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="55"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="I15" s="48"/>
-    </row>
-    <row r="16" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="24"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-    </row>
-    <row r="17" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="29"/>
-      <c r="C17" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-    </row>
-    <row r="19" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="47" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="53"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="48"/>
-    </row>
-    <row r="22" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="31"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-    </row>
-    <row r="23" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="29"/>
-      <c r="C23" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-    </row>
-    <row r="25" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-    </row>
-    <row r="27" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="49"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-    </row>
-    <row r="28" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="32"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-    </row>
-    <row r="29" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="29"/>
-      <c r="C29" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="C8:C9"/>
+  <mergeCells count="15">
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="H16:H17"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0.39370078740157483" footer="0.39370078740157483"/>
-  <pageSetup paperSize="9" scale="85" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="84" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dodanie do raportu sumy kontrolnej pliku
</commit_message>
<xml_diff>
--- a/raport/szablon_raport_importu.xlsx
+++ b/raport/szablon_raport_importu.xlsx
@@ -77,9 +77,6 @@
     <t>Geodezyjna Ewidencja Sieci Uzbrojenia Terenu</t>
   </si>
   <si>
-    <t>Suma kontrolna (SHA-256):</t>
-  </si>
-  <si>
     <t>modyfikowane</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t xml:space="preserve">Data i czas importu: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suma kontrolna (SHA-256): </t>
   </si>
 </sst>
 </file>
@@ -827,50 +827,50 @@
     <xf numFmtId="0" fontId="21" fillId="30" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="18" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="18" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="18" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="18" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -962,7 +962,7 @@
         <xdr:cNvPr id="2" name="Obraz 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15A37402-D866-0FDD-4B11-9268CBD4FA76}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15A37402-D866-0FDD-4B11-9268CBD4FA76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1290,9 +1290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1317,7 +1315,7 @@
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1328,7 +1326,7 @@
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1339,7 +1337,7 @@
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1369,13 +1367,13 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="55" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="9" t="s">
@@ -1384,19 +1382,19 @@
       <c r="E8" s="10"/>
       <c r="F8" s="15"/>
       <c r="G8" s="16"/>
-      <c r="H8" s="48" t="s">
+      <c r="H8" s="45" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="44"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="47"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="56"/>
       <c r="D9" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>5</v>
@@ -1404,7 +1402,7 @@
       <c r="G9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="49"/>
+      <c r="H9" s="46"/>
     </row>
     <row r="10" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="35"/>
@@ -1451,13 +1449,13 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="46" t="s">
+      <c r="C16" s="55" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="9" t="s">
@@ -1466,19 +1464,19 @@
       <c r="E16" s="10"/>
       <c r="F16" s="15"/>
       <c r="G16" s="16"/>
-      <c r="H16" s="48" t="s">
+      <c r="H16" s="45" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="50"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="47"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>5</v>
@@ -1486,7 +1484,7 @@
       <c r="G17" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="49"/>
+      <c r="H17" s="46"/>
     </row>
     <row r="18" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
@@ -1533,13 +1531,13 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="56" t="s">
+      <c r="A24" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="57" t="s">
+      <c r="B24" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="46" t="s">
+      <c r="C24" s="55" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="9" t="s">
@@ -1548,19 +1546,19 @@
       <c r="E24" s="10"/>
       <c r="F24" s="15"/>
       <c r="G24" s="16"/>
-      <c r="H24" s="48" t="s">
+      <c r="H24" s="45" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="56"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="47"/>
+      <c r="A25" s="53"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="56"/>
       <c r="D25" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>5</v>
@@ -1568,7 +1566,7 @@
       <c r="G25" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="49"/>
+      <c r="H25" s="46"/>
     </row>
     <row r="26" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25"/>
@@ -1584,12 +1582,12 @@
       <c r="B27" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
     </row>
     <row r="28" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="39"/>
@@ -1611,17 +1609,17 @@
     </row>
     <row r="31" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="52" t="s">
+      <c r="A32" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="53" t="s">
+      <c r="B32" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="54" t="s">
+      <c r="C32" s="51" t="s">
         <v>7</v>
       </c>
       <c r="D32" s="29"/>
@@ -1631,9 +1629,9 @@
       <c r="H32" s="29"/>
     </row>
     <row r="33" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="52"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="55"/>
+      <c r="A33" s="49"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="52"/>
       <c r="D33" s="29"/>
       <c r="E33" s="29"/>
       <c r="F33" s="29"/>
@@ -1654,7 +1652,7 @@
       <c r="B35" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="58"/>
+      <c r="C35" s="44"/>
       <c r="D35" s="28"/>
       <c r="E35" s="28"/>
       <c r="F35" s="28"/>
@@ -1663,6 +1661,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="H16:H17"/>
     <mergeCell ref="H24:H25"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
@@ -1672,12 +1676,6 @@
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="H16:H17"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0.39370078740157483" footer="0.39370078740157483"/>
   <pageSetup paperSize="9" scale="84" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
przywrocenie dodawania obowiazkowych pol, dodanie przycisku donate, poprawki wizualne w formatkach, dodanie prezentacji graficznej do pomocniczych
</commit_message>
<xml_diff>
--- a/raport/szablon_raport_importu.xlsx
+++ b/raport/szablon_raport_importu.xlsx
@@ -47,15 +47,9 @@
 obiektów</t>
   </si>
   <si>
-    <t>pierwsze</t>
-  </si>
-  <si>
     <t>archiwalne</t>
   </si>
   <si>
-    <t>zamknięte</t>
-  </si>
-  <si>
     <t>Liczba obiektów</t>
   </si>
   <si>
@@ -90,6 +84,12 @@
   </si>
   <si>
     <t xml:space="preserve">Suma kontrolna (SHA-256): </t>
+  </si>
+  <si>
+    <t>nowe (pierwsze)</t>
+  </si>
+  <si>
+    <t>usunięte (ostatnie)</t>
   </si>
 </sst>
 </file>
@@ -696,7 +696,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -734,9 +734,6 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="18" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -830,6 +827,18 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="22" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -860,16 +869,10 @@
     <xf numFmtId="0" fontId="1" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="18" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -953,7 +956,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>387568</xdr:colOff>
+      <xdr:colOff>240424</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>8540</xdr:rowOff>
     </xdr:to>
@@ -962,7 +965,7 @@
         <xdr:cNvPr id="2" name="Obraz 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15A37402-D866-0FDD-4B11-9268CBD4FA76}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15A37402-D866-0FDD-4B11-9268CBD4FA76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1296,26 +1299,28 @@
   <cols>
     <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="11.6640625" style="3" customWidth="1"/>
-    <col min="5" max="8" width="11.6640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="3" customWidth="1"/>
+    <col min="5" max="7" width="13.77734375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="8" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="16"/>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1326,7 +1331,7 @@
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1337,7 +1342,7 @@
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1350,14 +1355,14 @@
       <c r="D6" s="3"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="19" t="s">
-        <v>9</v>
+      <c r="G6" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1367,46 +1372,46 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="46" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E8" s="10"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="45" t="s">
-        <v>7</v>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="48" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="57"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="13" t="s">
+      <c r="A9" s="44"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="46"/>
+      <c r="G9" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="49"/>
     </row>
     <row r="10" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
@@ -1419,82 +1424,82 @@
         <v>2</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
     </row>
     <row r="12" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="41"/>
+      <c r="B13" s="40"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
     </row>
     <row r="15" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="55" t="s">
+      <c r="C16" s="46" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E16" s="10"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="45" t="s">
-        <v>7</v>
+      <c r="F16" s="14"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="48" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="47"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="13" t="s">
+      <c r="A17" s="50"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" s="46"/>
+      <c r="G17" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="49"/>
     </row>
     <row r="18" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
     </row>
     <row r="19" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
@@ -1508,165 +1513,159 @@
       <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="39"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
     </row>
     <row r="21" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="42"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
     </row>
     <row r="23" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="53" t="s">
+      <c r="A24" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="46" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E24" s="10"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="45" t="s">
-        <v>7</v>
+      <c r="F24" s="14"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="48" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="53"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="13" t="s">
+      <c r="A25" s="56"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25" s="46"/>
+      <c r="G25" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="49"/>
     </row>
     <row r="26" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="25"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
     </row>
     <row r="27" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
     </row>
     <row r="28" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="39"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
     </row>
     <row r="29" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="43"/>
+      <c r="B29" s="42"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
     </row>
     <row r="31" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="49" t="s">
+      <c r="A32" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="50" t="s">
+      <c r="B32" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="C32" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
     </row>
     <row r="33" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="49"/>
-      <c r="B33" s="50"/>
-      <c r="C33" s="52"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
     </row>
     <row r="34" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="26"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
     </row>
     <row r="35" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="H16:H17"/>
     <mergeCell ref="H24:H25"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
@@ -1676,6 +1675,12 @@
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="H16:H17"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0.39370078740157483" footer="0.39370078740157483"/>
   <pageSetup paperSize="9" scale="84" orientation="portrait" r:id="rId1"/>

</xml_diff>